<commit_message>
Genetic Algorithm and Results are updated
</commit_message>
<xml_diff>
--- a/sonuclar.xlsx
+++ b/sonuclar.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="87">
   <si>
     <t xml:space="preserve">SYN FLOOD VERISETI – 31 Dakikalik trafik %25 Saldiri Orani</t>
   </si>
@@ -67,10 +67,16 @@
     <t xml:space="preserve">IQR: 2.0</t>
   </si>
   <si>
+    <t xml:space="preserve">MATRIX_PROFILE_ISOLATION_FOREST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SK: 10 KTS:10</t>
+  </si>
+  <si>
     <t xml:space="preserve">LMOMS_SKEW_KURTOSIS</t>
   </si>
   <si>
-    <t xml:space="preserve">SK: 10 KTS:10</t>
+    <t xml:space="preserve">EST:100 CONT:AUTO</t>
   </si>
   <si>
     <t xml:space="preserve">SYN FLOOD + NTP VERISETI - 31 Dakikalik Trafik %25 Saldiri Orani</t>
@@ -85,6 +91,9 @@
     <t xml:space="preserve">IQR: 1.0</t>
   </si>
   <si>
+    <t xml:space="preserve">EST:50 CONT:AUTO</t>
+  </si>
+  <si>
     <t xml:space="preserve">Total Fwd Packets</t>
   </si>
   <si>
@@ -101,6 +110,322 @@
   </si>
   <si>
     <t xml:space="preserve">IQR:2.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EST:50 CONT:0.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Simulation Duration: 27756 Seconds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MP CALCULATION: CLASSIC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">' Total Fwd Packets'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Genetic Algorithm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FEATURES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">' Total Backward Packets'</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Population Bag Size: </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">10</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">5, 6, 16, 12, 7, 14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">' Total Length of Bwd Packets'</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Max Features: </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">20</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">14, 6, 16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">' Fwd Packet Length Min'</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Generation Size: </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">50</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">14, 19, 0, 18, 13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">' Fwd Packet Length Std'</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">CostFunction: </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">maximize f1 score</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">' Bwd Packet Length Min'</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Crossover Ratio: </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&lt;= 70</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">' Bwd Packet Length Std'</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Mutation Ratio: </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&lt;= 50</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">' Bwd Header Length'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">' Min Packet Length'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">' Packet Length Std'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">' SYN Flag Count'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">' ACK Flag Count'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Total Length of Fwd Packets'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ' Fwd Packet Length Max'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ' Fwd Packet Length Mean'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Bwd Packet Length Max'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ' Bwd Packet Length Mean'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ' Fwd Header Length'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Fwd Packets/s'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ' Max Packet Length'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ' Packet Length Variance'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ' RST Flag Count'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ' Bwd Packets/s'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ' Packet Length Mean'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'FIN Flag Count'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ' PSH Flag Count'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Simulation Duration: 1200 Seconds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MP CALCULATION: NOT CLASSIC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11, 19, 1, 3, 9, 5</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Max Features: </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">25</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">9, 6, 5</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Generation Size: </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">500</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">UNBW EXPLOIT (ZERO_DAY) ATTACK DATASET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ataklar saniye cinsinden degil FLOW Based </t>
+  </si>
+  <si>
+    <t xml:space="preserve">dijt/sinpkt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">response_body_len
+ct_dst_sport_ltm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percentile:70</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sload/dload</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iqr:1.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">response_body_len </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nest:100 cont: 0.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ct_srv_dst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sk: 10 kts: 10</t>
   </si>
 </sst>
 </file>
@@ -110,11 +435,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -136,9 +462,15 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -161,6 +493,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF81D41A"/>
         <bgColor rgb="FF969696"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFAA95"/>
+        <bgColor rgb="FFFFCC99"/>
       </patternFill>
     </fill>
   </fills>
@@ -198,12 +536,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -215,12 +553,32 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -271,7 +629,7 @@
       <rgbColor rgb="FFCCFFCC"/>
       <rgbColor rgb="FFFFFF99"/>
       <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFFFAA95"/>
       <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
@@ -306,9 +664,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>5165640</xdr:colOff>
+      <xdr:colOff>5164920</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>73440</xdr:rowOff>
+      <xdr:rowOff>72720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -321,8 +679,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1641600" y="1463400"/>
-          <a:ext cx="5149800" cy="2836440"/>
+          <a:off x="1646640" y="1463400"/>
+          <a:ext cx="5149080" cy="2835720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -343,9 +701,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>4964760</xdr:colOff>
+      <xdr:colOff>4964040</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>19080</xdr:rowOff>
+      <xdr:rowOff>18360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -358,8 +716,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1487160" y="4962600"/>
-          <a:ext cx="5103360" cy="2859480"/>
+          <a:off x="1489680" y="4962600"/>
+          <a:ext cx="5105160" cy="2858760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -380,9 +738,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>5121000</xdr:colOff>
+      <xdr:colOff>5120280</xdr:colOff>
       <xdr:row>68</xdr:row>
-      <xdr:rowOff>57240</xdr:rowOff>
+      <xdr:rowOff>56520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -395,8 +753,119 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1625760" y="8290800"/>
-          <a:ext cx="5121000" cy="2820600"/>
+          <a:off x="1630800" y="8290800"/>
+          <a:ext cx="5120280" cy="2819880"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>10080</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>153360</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>5130360</xdr:colOff>
+      <xdr:row>107</xdr:row>
+      <xdr:rowOff>47160</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Image 4" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId4"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1640880" y="14621040"/>
+          <a:ext cx="5120280" cy="2819880"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>153</xdr:row>
+      <xdr:rowOff>9000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>5072040</xdr:colOff>
+      <xdr:row>174</xdr:row>
+      <xdr:rowOff>69480</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Image 5" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId5"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1630800" y="24880680"/>
+          <a:ext cx="5072040" cy="3614400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>10080</xdr:colOff>
+      <xdr:row>124</xdr:row>
+      <xdr:rowOff>153000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>5130360</xdr:colOff>
+      <xdr:row>142</xdr:row>
+      <xdr:rowOff>46800</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Image 4" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId6"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1640880" y="20310480"/>
+          <a:ext cx="5120280" cy="2819880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -416,18 +885,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="C9:I62"/>
+  <dimension ref="C9:L159"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A18" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A94" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G122" activeCellId="0" sqref="G122"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="73.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="33.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="36.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="29.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="34.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="26.53"/>
   </cols>
   <sheetData>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -475,7 +947,7 @@
         <v>9</v>
       </c>
       <c r="H13" s="0" t="n">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I13" s="0" t="n">
         <v>90</v>
@@ -495,10 +967,10 @@
         <v>11</v>
       </c>
       <c r="H14" s="0" t="n">
-        <v>96</v>
-      </c>
-      <c r="I14" s="2" t="n">
         <v>94</v>
+      </c>
+      <c r="I14" s="3" t="n">
+        <v>92</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -518,11 +990,11 @@
         <v>72</v>
       </c>
       <c r="I15" s="0" t="n">
-        <v>30</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="0" t="s">
         <v>15</v>
       </c>
       <c r="E16" s="0" t="s">
@@ -534,16 +1006,36 @@
       <c r="G16" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="H16" s="2" t="n">
-        <v>96</v>
-      </c>
-      <c r="I16" s="2" t="n">
-        <v>94</v>
+      <c r="H16" s="3" t="n">
+        <v>73</v>
+      </c>
+      <c r="I16" s="3" t="n">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D17" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F17" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="G17" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="H17" s="2" t="n">
+        <v>95</v>
+      </c>
+      <c r="I17" s="2" t="n">
+        <v>93</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C30" s="4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
@@ -589,7 +1081,7 @@
         <v>89</v>
       </c>
       <c r="I34" s="0" t="n">
-        <v>81</v>
+        <v>84</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -597,19 +1089,19 @@
         <v>10</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F35" s="0" t="n">
         <v>20</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="H35" s="0" t="n">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I35" s="0" t="n">
-        <v>81</v>
+        <v>85</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -623,38 +1115,62 @@
         <v>20</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H36" s="0" t="n">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I36" s="0" t="n">
-        <v>80</v>
+        <v>86</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D37" s="3" t="s">
+      <c r="D37" s="0" t="s">
         <v>15</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="F37" s="0" t="n">
         <v>20</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="H37" s="2" t="n">
-        <v>93</v>
-      </c>
-      <c r="I37" s="2" t="n">
-        <v>87</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="H37" s="0" t="n">
+        <v>86</v>
+      </c>
+      <c r="I37" s="0" t="n">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D38" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E38" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="F38" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="G38" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="H38" s="2" t="n">
+        <v>92</v>
+      </c>
+      <c r="I38" s="2" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C51" s="5" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D51" s="5"/>
       <c r="E51" s="5"/>
@@ -697,10 +1213,10 @@
         <v>9</v>
       </c>
       <c r="H59" s="0" t="n">
-        <v>89</v>
-      </c>
-      <c r="I59" s="0" t="n">
-        <v>74</v>
+        <v>87</v>
+      </c>
+      <c r="I59" s="3" t="n">
+        <v>79</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -714,13 +1230,13 @@
         <v>20</v>
       </c>
       <c r="G60" s="0" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="H60" s="2" t="n">
-        <v>90</v>
-      </c>
-      <c r="I60" s="2" t="n">
-        <v>70</v>
+        <v>89</v>
+      </c>
+      <c r="I60" s="3" t="n">
+        <v>80</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -728,46 +1244,830 @@
         <v>12</v>
       </c>
       <c r="E61" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F61" s="0" t="n">
         <v>20</v>
       </c>
       <c r="G61" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="H61" s="0" t="n">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I61" s="0" t="n">
-        <v>69</v>
+        <v>82</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D62" s="3" t="s">
+      <c r="D62" s="0" t="s">
         <v>15</v>
       </c>
       <c r="E62" s="0" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="F62" s="0" t="n">
         <v>20</v>
       </c>
       <c r="G62" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="H62" s="0" t="n">
+        <v>88</v>
+      </c>
+      <c r="I62" s="0" t="n">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D63" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E63" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F63" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="G63" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="H62" s="2" t="n">
-        <v>90</v>
-      </c>
-      <c r="I62" s="2" t="n">
+      <c r="H63" s="0" t="n">
+        <v>89</v>
+      </c>
+      <c r="I63" s="2" t="n">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C80" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C81" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C82" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D82" s="6"/>
+      <c r="E82" s="6"/>
+      <c r="F82" s="6"/>
+      <c r="G82" s="6"/>
+      <c r="H82" s="6"/>
+      <c r="I82" s="6"/>
+      <c r="K82" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L82" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C83" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E83" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F83" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G83" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H83" s="2"/>
+      <c r="I83" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K83" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L83" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C84" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="D84" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E84" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="F84" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="G84" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="I84" s="0" t="n">
+        <v>69</v>
+      </c>
+      <c r="K84" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="L84" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C85" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="D85" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E85" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="F85" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="G85" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="I85" s="0" t="n">
+        <v>73</v>
+      </c>
+      <c r="K85" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="L85" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C86" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="D86" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E86" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="F86" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="G86" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="I86" s="2" t="n">
+        <v>82</v>
+      </c>
+      <c r="K86" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="L86" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C87" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="K87" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="L87" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C88" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="K88" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="L88" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C89" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="K89" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="L89" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K90" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="L90" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K91" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="L91" s="8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K92" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="L92" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K93" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="L93" s="8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K94" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="L94" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K95" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="L95" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K96" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="L96" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K97" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="L97" s="0" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K98" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="L98" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K99" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="L99" s="0" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K100" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="L100" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K101" s="2" t="n">
+        <v>19</v>
+      </c>
+      <c r="L101" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K102" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="L102" s="0" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K103" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="L103" s="0" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K104" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="L104" s="0" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K105" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="L105" s="0" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K106" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="L106" s="0" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K107" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="L107" s="0" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C115" s="0" t="s">
         <v>70</v>
       </c>
     </row>
+    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C116" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C117" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D117" s="6"/>
+      <c r="E117" s="6"/>
+      <c r="F117" s="6"/>
+      <c r="G117" s="6"/>
+      <c r="H117" s="6"/>
+      <c r="I117" s="6"/>
+      <c r="K117" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L117" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C118" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D118" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E118" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F118" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G118" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H118" s="2"/>
+      <c r="I118" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K118" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="L118" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C119" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="D119" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E119" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="F119" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="G119" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="I119" s="0" t="n">
+        <v>85</v>
+      </c>
+      <c r="K119" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="L119" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C120" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="D120" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E120" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="F120" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="G120" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="I120" s="0" t="n">
+        <v>82</v>
+      </c>
+      <c r="K120" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="L120" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C121" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="D121" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E121" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="F121" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="G121" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="I121" s="2" t="n">
+        <v>89</v>
+      </c>
+      <c r="K121" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="L121" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C122" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="D122" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="G122" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="K122" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="L122" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C123" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="K123" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="L123" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C124" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="K124" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="L124" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K125" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="L125" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K126" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="L126" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K127" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="L127" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K128" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="L128" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K129" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="L129" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K130" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="L130" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K131" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="L131" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K132" s="3" t="n">
+        <v>15</v>
+      </c>
+      <c r="L132" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K133" s="3" t="n">
+        <v>16</v>
+      </c>
+      <c r="L133" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K134" s="3" t="n">
+        <v>17</v>
+      </c>
+      <c r="L134" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K135" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="L135" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K136" s="2" t="n">
+        <v>19</v>
+      </c>
+      <c r="L136" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K137" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="L137" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K138" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="L138" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K139" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="L139" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K140" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="L140" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K141" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="L141" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K142" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="L142" s="0" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C150" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="D150" s="9"/>
+      <c r="E150" s="9"/>
+      <c r="F150" s="9"/>
+      <c r="G150" s="9"/>
+      <c r="H150" s="9"/>
+      <c r="I150" s="9"/>
+      <c r="J150" s="9"/>
+    </row>
+    <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C152" s="0" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D154" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E154" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F154" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G154" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H154" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I154" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D155" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E155" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="F155" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="G155" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="H155" s="0" t="n">
+        <v>77</v>
+      </c>
+      <c r="I155" s="0" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="156" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D156" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E156" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="F156" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="G156" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="H156" s="3" t="n">
+        <v>76</v>
+      </c>
+      <c r="I156" s="3" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D157" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E157" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="F157" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="G157" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="H157" s="0" t="n">
+        <v>76</v>
+      </c>
+      <c r="I157" s="3" t="n">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D158" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E158" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="F158" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="G158" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="H158" s="2" t="n">
+        <v>83</v>
+      </c>
+      <c r="I158" s="2" t="n">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D159" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E159" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="F159" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="G159" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="H159" s="0" t="n">
+        <v>71</v>
+      </c>
+      <c r="I159" s="3" t="n">
+        <v>61</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="6">
     <mergeCell ref="C9:I9"/>
     <mergeCell ref="C30:I30"/>
     <mergeCell ref="C51:I51"/>
+    <mergeCell ref="C82:I82"/>
+    <mergeCell ref="C117:I117"/>
+    <mergeCell ref="C150:J150"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>